<commit_message>
update log book, katakana,jade + burndown chart
</commit_message>
<xml_diff>
--- a/BurnDownChart.xlsx
+++ b/BurnDownChart.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="19020" windowHeight="8580"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -49,6 +49,30 @@
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>goodoldmanoj.com:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Remaining effort as of that day to complete the task. NOT last day effort - hours worked. So this can go up if new challenges got uncovered</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="0">
+      <text>
+        <r>
+          <rPr>
             <sz val="8"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
@@ -64,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>Project</t>
   </si>
@@ -173,12 +197,18 @@
   <si>
     <t>www.goodoldmanoj.com</t>
   </si>
+  <si>
+    <t>Day 11</t>
+  </si>
+  <si>
+    <t>Day 12</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,10 +310,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -293,12 +319,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -308,12 +338,27 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -332,11 +377,14 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -345,37 +393,40 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$5:$O$5</c:f>
+              <c:f>Sheet1!$G$5:$Q$5</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>Day 11</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Day 10</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Day 9</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Day 8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Day 7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Day 6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Day 5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Day 4</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Day 3</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Day 2</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Day 1</c:v>
                 </c:pt>
               </c:strCache>
@@ -420,6 +471,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -429,37 +481,40 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$5:$O$5</c:f>
+              <c:f>Sheet1!$G$5:$Q$5</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>Day 11</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Day 10</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Day 9</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Day 8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Day 7</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Day 6</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>Day 5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Day 4</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Day 3</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Day 2</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Day 1</c:v>
                 </c:pt>
               </c:strCache>
@@ -489,38 +544,50 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
+          <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="59776384"/>
-        <c:axId val="59778560"/>
+        <c:smooth val="0"/>
+        <c:axId val="78058240"/>
+        <c:axId val="78059776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59776384"/>
+        <c:axId val="78058240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59778560"/>
+        <c:crossAx val="78059776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59778560"/>
+        <c:axId val="78059776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="59776384"/>
+        <c:crossAx val="78058240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -528,8 +595,11 @@
     <c:legend>
       <c:legendPos val="t"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -858,21 +928,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="7" customFormat="1" ht="15.75">
+    <row r="1" spans="1:16384" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -17260,7 +17330,7 @@
       <c r="XFC1" s="1"/>
       <c r="XFD1" s="1"/>
     </row>
-    <row r="2" spans="1:16384" s="8" customFormat="1" ht="17.25" customHeight="1">
+    <row r="2" spans="1:16384" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -33646,18 +33716,18 @@
       <c r="XFC2" s="1"/>
       <c r="XFD2" s="1"/>
     </row>
-    <row r="3" spans="1:16384" s="7" customFormat="1" ht="23.25">
+    <row r="3" spans="1:16384" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -50034,7 +50104,7 @@
       <c r="XFC3" s="1"/>
       <c r="XFD3" s="1"/>
     </row>
-    <row r="4" spans="1:16384">
+    <row r="4" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -50055,610 +50125,614 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:16384">
+    <row r="5" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="K5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="L5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="M5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="N5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="O5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="P5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="Q5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:16384">
+    <row r="6" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>8</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>4</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>0</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>0</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>0</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <v>0</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:16384">
+    <row r="7" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>6</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>2</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>3</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>5</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>2</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <v>0</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:16384">
+    <row r="8" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>5</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>5</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>3</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>2</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>2</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <v>0</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:16384">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>8</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>8</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>8</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>8</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>7</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="4">
         <v>3</v>
       </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:16384">
+    <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>8</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>8</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>8</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>8</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>8</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="4">
         <v>7</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:16384">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>9</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>9</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>9</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>9</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <v>9</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="4">
         <v>9</v>
       </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:16384">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>5</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>5</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>5</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="4">
         <v>5</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="4">
         <v>5</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="4">
         <v>5</v>
       </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:16384">
+    <row r="13" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>7</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>7</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <v>7</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="4">
         <v>7</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="4">
         <v>7</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="4">
         <v>7</v>
       </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:16384">
+    <row r="14" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>3</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>3</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <v>3</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="4">
         <v>3</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="4">
         <v>3</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="4">
         <v>3</v>
       </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:16384">
+    <row r="15" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>8</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>8</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <v>8</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="4">
         <v>8</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="4">
         <v>8</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="4">
         <v>8</v>
       </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:16384">
+    <row r="16" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>6</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <v>6</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <v>6</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="4">
         <v>6</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="4">
         <v>6</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="4">
         <v>6</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>8</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <v>8</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <v>8</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="4">
         <v>8</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="4">
         <v>8</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J17" s="4">
         <v>8</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>9</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <v>9</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <v>9</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="4">
         <v>9</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="4">
         <v>9</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="4">
         <v>9</v>
       </c>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="5">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="4">
         <f>SUM(E6:E18)</f>
         <v>90</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <f>E19-$E$19/10</f>
         <v>81</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <f t="shared" ref="G19:O19" si="0">F19-$E$19/10</f>
         <v>72</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="4">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="4">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="J19" s="5">
+      <c r="J19" s="4">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19" s="4">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="L19" s="5">
+      <c r="L19" s="4">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="M19" s="5">
+      <c r="M19" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="N19" s="5">
+      <c r="N19" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="O19" s="5">
+      <c r="O19" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -50667,48 +50741,48 @@
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="5">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="4">
         <f>SUM(E6:E18)</f>
         <v>90</v>
       </c>
-      <c r="F20" s="5">
-        <f t="shared" ref="F20:O20" si="1">SUM(F6:F18)</f>
+      <c r="F20" s="4">
+        <f t="shared" ref="F20:J20" si="1">SUM(F6:F18)</f>
         <v>82</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="4">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="4">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="J20" s="5">
+      <c r="J20" s="4">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -50729,7 +50803,7 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -50750,7 +50824,7 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -50771,7 +50845,7 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -50792,7 +50866,7 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -50813,7 +50887,7 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -50834,7 +50908,7 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -50855,7 +50929,7 @@
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -50876,7 +50950,7 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -50897,7 +50971,7 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -50918,7 +50992,7 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -50939,7 +51013,7 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -50960,7 +51034,7 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -50981,7 +51055,7 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -51002,7 +51076,7 @@
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -51023,7 +51097,7 @@
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -51044,7 +51118,7 @@
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -51065,7 +51139,7 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
     </row>
-    <row r="38" spans="1:19">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -51086,7 +51160,7 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -51107,7 +51181,7 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -51128,7 +51202,7 @@
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -51149,7 +51223,7 @@
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -51170,7 +51244,7 @@
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -51191,7 +51265,7 @@
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
     </row>
-    <row r="44" spans="1:19">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -51212,7 +51286,7 @@
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
     </row>
-    <row r="45" spans="1:19">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -51233,7 +51307,7 @@
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
     </row>
-    <row r="46" spans="1:19">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -51254,7 +51328,7 @@
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -51275,7 +51349,7 @@
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
     </row>
-    <row r="48" spans="1:19">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -51296,7 +51370,7 @@
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -51317,7 +51391,7 @@
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
     </row>
-    <row r="50" spans="1:19">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -51338,7 +51412,7 @@
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -51359,7 +51433,7 @@
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -51380,7 +51454,7 @@
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
     </row>
-    <row r="53" spans="1:19">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -51401,7 +51475,7 @@
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
     </row>
-    <row r="54" spans="1:19">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -51422,7 +51496,7 @@
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
     </row>
-    <row r="55" spans="1:19">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -51443,7 +51517,7 @@
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
     </row>
-    <row r="56" spans="1:19">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -51483,24 +51557,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>